<commit_message>
Fix lint error and add Firebase config
</commit_message>
<xml_diff>
--- a/Sky5_Kitchen_Admin_Kit.xlsx
+++ b/Sky5_Kitchen_Admin_Kit.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Master Menu" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Daily SOP Checklist" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sales Register" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Staff Attendance" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -32,7 +33,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +58,12 @@
         <bgColor rgb="0024963F"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -70,7 +77,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -79,6 +86,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1750,4 +1760,726 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="17" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Employee Name</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Check-In Time</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Check-Out Time</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Total Hours</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Daily Wage (INR)</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Total Pay (INR)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>EMP-001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Staff Member 1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G2">
+        <f>(F2-E2)*24</f>
+        <v/>
+      </c>
+      <c r="H2" t="n">
+        <v>500</v>
+      </c>
+      <c r="I2">
+        <f>G2*H2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>EMP-002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Staff Member 2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G3">
+        <f>(F3-E3)*24</f>
+        <v/>
+      </c>
+      <c r="H3" t="n">
+        <v>500</v>
+      </c>
+      <c r="I3">
+        <f>G3*H3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>EMP-003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Staff Member 3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G4">
+        <f>(F4-E4)*24</f>
+        <v/>
+      </c>
+      <c r="H4" t="n">
+        <v>500</v>
+      </c>
+      <c r="I4">
+        <f>G4*H4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EMP-004</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Staff Member 4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G5">
+        <f>(F5-E5)*24</f>
+        <v/>
+      </c>
+      <c r="H5" t="n">
+        <v>500</v>
+      </c>
+      <c r="I5">
+        <f>G5*H5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>EMP-005</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Staff Member 5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G6">
+        <f>(F6-E6)*24</f>
+        <v/>
+      </c>
+      <c r="H6" t="n">
+        <v>500</v>
+      </c>
+      <c r="I6">
+        <f>G6*H6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EMP-006</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Staff Member 6</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G7">
+        <f>(F7-E7)*24</f>
+        <v/>
+      </c>
+      <c r="H7" t="n">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <f>G7*H7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>EMP-007</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Staff Member 7</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G8">
+        <f>(F8-E8)*24</f>
+        <v/>
+      </c>
+      <c r="H8" t="n">
+        <v>500</v>
+      </c>
+      <c r="I8">
+        <f>G8*H8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EMP-008</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Staff Member 8</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G9">
+        <f>(F9-E9)*24</f>
+        <v/>
+      </c>
+      <c r="H9" t="n">
+        <v>500</v>
+      </c>
+      <c r="I9">
+        <f>G9*H9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>EMP-009</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Staff Member 9</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G10">
+        <f>(F10-E10)*24</f>
+        <v/>
+      </c>
+      <c r="H10" t="n">
+        <v>500</v>
+      </c>
+      <c r="I10">
+        <f>G10*H10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EMP-010</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Staff Member 10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G11">
+        <f>(F11-E11)*24</f>
+        <v/>
+      </c>
+      <c r="H11" t="n">
+        <v>500</v>
+      </c>
+      <c r="I11">
+        <f>G11*H11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>EMP-011</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Staff Member 11</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G12">
+        <f>(F12-E12)*24</f>
+        <v/>
+      </c>
+      <c r="H12" t="n">
+        <v>500</v>
+      </c>
+      <c r="I12">
+        <f>G12*H12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>EMP-012</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Staff Member 12</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G13">
+        <f>(F13-E13)*24</f>
+        <v/>
+      </c>
+      <c r="H13" t="n">
+        <v>500</v>
+      </c>
+      <c r="I13">
+        <f>G13*H13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>EMP-013</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Staff Member 13</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G14">
+        <f>(F14-E14)*24</f>
+        <v/>
+      </c>
+      <c r="H14" t="n">
+        <v>500</v>
+      </c>
+      <c r="I14">
+        <f>G14*H14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>EMP-014</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Staff Member 14</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G15">
+        <f>(F15-E15)*24</f>
+        <v/>
+      </c>
+      <c r="H15" t="n">
+        <v>500</v>
+      </c>
+      <c r="I15">
+        <f>G15*H15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EMP-015</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Staff Member 15</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="G16">
+        <f>(F16-E16)*24</f>
+        <v/>
+      </c>
+      <c r="H16" t="n">
+        <v>500</v>
+      </c>
+      <c r="I16">
+        <f>G16*H16</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>